<commit_message>
intermediate work with JOS
</commit_message>
<xml_diff>
--- a/OTPL Manufaturing App.xlsx
+++ b/OTPL Manufaturing App.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916487B9-764B-49FC-A63E-BFF511313BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{103956A6-528F-49F6-AD84-8A2EF6D8FBC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="50">
   <si>
     <t>Image</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>Stages for manufacturing of order ---&gt; Whatsapp notification can be sent to manufacturer to update the process stage</t>
+  </si>
+  <si>
+    <t>\</t>
   </si>
 </sst>
 </file>
@@ -681,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C1:AO23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="L4" workbookViewId="0">
+      <selection activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1533,6 +1536,9 @@
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="8"/>
+      <c r="AF21" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="22" spans="3:39" x14ac:dyDescent="0.35">
       <c r="C22" s="6"/>
@@ -1562,7 +1568,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E72B996-2BB4-4096-9002-9BF61C0C677E}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>